<commit_message>
Updated Cal and Ingest Sheets
Calibration sheets have been updated as per emails from Steve Gaul and
Joe Lofgren. Ingestion CSVs for CP02 platforms have also been updated to
fix a bad reference designator.
</commit_message>
<xml_diff>
--- a/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00002.xlsx
+++ b/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12405" tabRatio="377"/>
+    <workbookView xWindow="12708" yWindow="-12" windowWidth="12516" windowHeight="12408" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,12 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$84</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$400</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>Ref Des</t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>CE09OSPM-SBS01-00-STCENG000</t>
-  </si>
-  <si>
-    <t>Complete</t>
   </si>
   <si>
     <t>CE09OSPM-00002</t>
@@ -834,27 +831,27 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.85546875"/>
-    <col min="2" max="2" width="39.42578125"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125"/>
-    <col min="7" max="7" width="18.7109375"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875"/>
-    <col min="10" max="10" width="12.7109375"/>
-    <col min="11" max="11" width="51.7109375"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="1026" width="8.7109375"/>
+    <col min="1" max="1" width="37.88671875"/>
+    <col min="2" max="2" width="39.44140625"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.44140625"/>
+    <col min="7" max="7" width="18.6640625"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875"/>
+    <col min="10" max="10" width="12.6640625"/>
+    <col min="11" max="11" width="51.6640625"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="1026" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5">
+    <row r="1" spans="1:13" ht="31.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,12 +886,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="15">
       <c r="A2" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="15">
         <v>2</v>
@@ -907,16 +904,16 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>43</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>44</v>
       </c>
       <c r="I2" s="5">
         <v>542</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="23">
@@ -933,9 +930,6 @@
       <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
@@ -953,22 +947,22 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125"/>
-    <col min="8" max="8" width="11.85546875"/>
-    <col min="9" max="9" width="14.42578125"/>
-    <col min="10" max="10" width="13.42578125"/>
-    <col min="11" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625"/>
+    <col min="8" max="8" width="11.88671875"/>
+    <col min="9" max="9" width="14.44140625"/>
+    <col min="10" max="10" width="13.44140625"/>
+    <col min="11" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +987,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="9">
         <v>2</v>
@@ -1013,7 +1007,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="9">
         <v>2</v>
@@ -1033,7 +1027,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="9">
         <v>2</v>
@@ -1053,7 +1047,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="9">
         <v>2</v>
@@ -1073,7 +1067,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9">
         <v>2</v>
@@ -1093,7 +1087,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -1113,7 +1107,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="9">
         <v>2</v>
@@ -1133,7 +1127,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="9">
         <v>2</v>
@@ -1161,7 +1155,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
@@ -1181,7 +1175,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
@@ -1206,10 +1200,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
@@ -1226,10 +1220,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="9">
         <v>2</v>
@@ -1257,7 +1251,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="9">
         <v>2</v>
@@ -1266,7 +1260,7 @@
         <v>1032</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="19">
         <v>1.08</v>
@@ -1277,7 +1271,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="9">
         <v>2</v>
@@ -1297,7 +1291,7 @@
         <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
@@ -1317,7 +1311,7 @@
         <v>36</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="9">
         <v>2</v>
@@ -1337,7 +1331,7 @@
         <v>36</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -1346,7 +1340,7 @@
         <v>1032</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" s="19">
         <v>3.9E-2</v>
@@ -1357,7 +1351,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -1366,7 +1360,7 @@
         <v>1032</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" s="19">
         <v>700</v>
@@ -1377,7 +1371,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="9">
         <v>2</v>
@@ -1397,7 +1391,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="9">
         <v>2</v>
@@ -1417,7 +1411,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="9">
         <v>2</v>
@@ -1437,7 +1431,7 @@
         <v>36</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="9">
         <v>2</v>
@@ -1446,7 +1440,7 @@
         <v>1032</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="19">
         <v>117</v>
@@ -1465,7 +1459,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="9">
         <v>2</v>
@@ -1485,7 +1479,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="9">
         <v>2</v>
@@ -1508,47 +1502,47 @@
         <v>38</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="9">
         <v>2</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="9">
         <v>2</v>
       </c>
       <c r="D32" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="26" t="s">
         <v>52</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="9">
         <v>2</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>